<commit_message>
edited excel file row widths for image
</commit_message>
<xml_diff>
--- a/BaltimoreCity_Citations_Processed/BaltimoreCity_citations_processed.xlsx
+++ b/BaltimoreCity_Citations_Processed/BaltimoreCity_citations_processed.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -113,9 +113,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -168,12 +165,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,15 +470,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -489,7 +496,7 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>44617</v>
       </c>
       <c r="C2" t="s">
@@ -500,7 +507,7 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>44673</v>
       </c>
       <c r="C3" t="s">
@@ -511,7 +518,7 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>44687</v>
       </c>
       <c r="C4" t="s">
@@ -522,7 +529,7 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>44705</v>
       </c>
       <c r="C5" t="s">
@@ -533,7 +540,7 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>44711</v>
       </c>
       <c r="C6" t="s">
@@ -544,7 +551,7 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>44724</v>
       </c>
       <c r="C7" t="s">
@@ -555,7 +562,7 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>44724</v>
       </c>
       <c r="C8" t="s">
@@ -566,7 +573,7 @@
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <v>44729</v>
       </c>
       <c r="C9" t="s">
@@ -577,7 +584,7 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>44734</v>
       </c>
       <c r="C10" t="s">
@@ -588,7 +595,7 @@
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="3">
         <v>44737</v>
       </c>
       <c r="C11" t="s">
@@ -599,7 +606,7 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="3">
         <v>44743</v>
       </c>
       <c r="C12" t="s">
@@ -610,7 +617,7 @@
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="3">
         <v>44743</v>
       </c>
       <c r="C13" t="s">
@@ -621,7 +628,7 @@
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="3">
         <v>44743</v>
       </c>
       <c r="C14" t="s">
@@ -632,7 +639,7 @@
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <v>44743</v>
       </c>
       <c r="C15" t="s">
@@ -643,7 +650,7 @@
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="3">
         <v>44743</v>
       </c>
       <c r="C16" t="s">
@@ -654,7 +661,7 @@
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="3">
         <v>44743</v>
       </c>
       <c r="C17" t="s">
@@ -665,7 +672,7 @@
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="3">
         <v>44753</v>
       </c>
       <c r="C18" t="s">
@@ -676,7 +683,7 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="3">
         <v>44757</v>
       </c>
       <c r="C19" t="s">
@@ -687,7 +694,7 @@
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="3">
         <v>44757</v>
       </c>
       <c r="C20" t="s">
@@ -698,7 +705,7 @@
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="3">
         <v>44770</v>
       </c>
       <c r="C21" t="s">
@@ -709,7 +716,7 @@
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="3">
         <v>44774</v>
       </c>
       <c r="C22" t="s">
@@ -720,7 +727,7 @@
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="3">
         <v>44777</v>
       </c>
       <c r="C23" t="s">
@@ -731,7 +738,7 @@
       <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="3">
         <v>44778</v>
       </c>
       <c r="C24" t="s">
@@ -742,7 +749,7 @@
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="3">
         <v>44778</v>
       </c>
       <c r="C25" t="s">
@@ -753,7 +760,7 @@
       <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="3">
         <v>44784</v>
       </c>
       <c r="C26" t="s">
@@ -764,7 +771,7 @@
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="3">
         <v>44785</v>
       </c>
       <c r="C27" t="s">
@@ -775,7 +782,7 @@
       <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="3">
         <v>44785</v>
       </c>
       <c r="C28" t="s">
@@ -784,5 +791,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>